<commit_message>
Updated buckling safety factor
</commit_message>
<xml_diff>
--- a/FrontVD.xlsx
+++ b/FrontVD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\timot\Documents\Projects\Git\Wishbone-Forces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AC29D8-6BB7-44EE-9F99-62371E0315D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C053B2-C9F2-478F-B6CA-26CA0AB7F112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1061,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1829,7 +1829,8 @@
         <v>5</v>
       </c>
       <c r="I20" s="3">
-        <v>5</v>
+        <f>15/16*25.4</f>
+        <v>23.8125</v>
       </c>
       <c r="J20" s="3">
         <v>5</v>
@@ -1858,28 +1859,28 @@
         <v>42</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" ref="G21:L21" si="0">-G14*(G19/1000)^2/(PI()^2*$C$17)</f>
-        <v>3.1005094521903652E-11</v>
+        <f>-G14*(G19/1000)^2/(PI()^2*$C$17/$C$20)</f>
+        <v>6.2010189043807304E-11</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="0"/>
-        <v>2.3382680583549055E-11</v>
+        <f t="shared" ref="H21:L21" si="0">-H14*(H19/1000)^2/(PI()^2*$C$17/$C$20)</f>
+        <v>4.676536116709811E-11</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" si="0"/>
-        <v>1.2590205903338838E-10</v>
+        <v>2.5180411806677675E-10</v>
       </c>
       <c r="J21" s="5">
         <f t="shared" si="0"/>
-        <v>2.7918631189571309E-10</v>
+        <v>5.5837262379142617E-10</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="0"/>
-        <v>-1.5253114614422555E-10</v>
+        <v>-3.050622922884511E-10</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="0"/>
-        <v>4.4847410327122315E-11</v>
+        <v>8.9694820654244631E-11</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>43</v>
@@ -1897,19 +1898,19 @@
       </c>
       <c r="G22" s="7">
         <f t="shared" ref="G22:J22" si="1">IF(G21&gt;0,(2*G21*$C$20/PI()+(G20/1000)^4)^0.25*1000,"Tension only")</f>
-        <v>5.0771497602802311</v>
+        <v>5.1509346883040346</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="1"/>
-        <v>5.0585084988379609</v>
+        <v>5.1150544821929254</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="1"/>
-        <v>5.2937006684873298</v>
+        <v>23.818433837477802</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="1"/>
-        <v>5.5957550333866815</v>
+        <v>6.0457044082781692</v>
       </c>
       <c r="K22" s="7" t="str">
         <f>IF(K21&gt;0,(2*K21*$C$20/PI()+(K20/1000)^4)^0.25*1000,"Tension only")</f>
@@ -1917,7 +1918,7 @@
       </c>
       <c r="L22" s="7">
         <f>IF(L21&gt;0,(2*L21*$C$20/PI()+(L20/1000)^4)^0.25*1000,"Tension only")</f>
-        <v>5.110486560920287</v>
+        <v>5.2142389457909761</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
@@ -1966,7 +1967,7 @@
       </c>
       <c r="I24" s="7">
         <f t="shared" si="3"/>
-        <v>7.2616875999537642</v>
+        <v>24.387850726321133</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="3"/>
@@ -1998,11 +1999,11 @@
       </c>
       <c r="I25" s="8">
         <f t="shared" si="4"/>
-        <v>7.2616875999537642</v>
+        <v>24.387850726321133</v>
       </c>
       <c r="J25" s="8">
         <f t="shared" si="4"/>
-        <v>5.5957550333866815</v>
+        <v>6.0457044082781692</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="4"/>
@@ -2051,6 +2052,12 @@
       <c r="N28" s="6">
         <f t="shared" si="5"/>
         <v>9399.5730410906199</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <f>((I25-I20)/25.4)^-1</f>
+        <v>44.146985200506954</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for new forces
</commit_message>
<xml_diff>
--- a/FrontVD.xlsx
+++ b/FrontVD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\timot\Documents\Projects\Git\Wishbone-Forces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922ADCB3-5213-4141-B355-1ABFA2A77182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49B75D7-5978-4F1D-9B25-AA23A1658D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="7956" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FrontVD V2" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Scenario</t>
   </si>
@@ -80,36 +80,18 @@
     <t>Brake</t>
   </si>
   <si>
-    <t>Bump</t>
-  </si>
-  <si>
-    <t>Brake Bump</t>
-  </si>
-  <si>
     <t xml:space="preserve">Corner Outside </t>
   </si>
   <si>
     <t>Corner Outside Brake</t>
   </si>
   <si>
-    <t>Corner Outside Bump</t>
-  </si>
-  <si>
-    <t>Corner Outside Brake Bump</t>
-  </si>
-  <si>
     <t xml:space="preserve">Corner Inside </t>
   </si>
   <si>
     <t>Corner Inside Brake</t>
   </si>
   <si>
-    <t>Corner Inner Bump</t>
-  </si>
-  <si>
-    <t>Corner Inner Brake Bump</t>
-  </si>
-  <si>
     <t>Max compression</t>
   </si>
   <si>
@@ -189,12 +171,63 @@
   </si>
   <si>
     <t>Critical Thickness/mm</t>
+  </si>
+  <si>
+    <t>Critical Thickness/in</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Brake Impact</t>
+  </si>
+  <si>
+    <t>Corner Outside Impact</t>
+  </si>
+  <si>
+    <t>Corner Outside Brake Impact</t>
+  </si>
+  <si>
+    <t>Corner Inner Impact</t>
+  </si>
+  <si>
+    <t>Corner Inner Brake Impact</t>
+  </si>
+  <si>
+    <t>Full squat</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>20SWG</t>
+  </si>
+  <si>
+    <t>.036"</t>
+  </si>
+  <si>
+    <t>16SWG</t>
+  </si>
+  <si>
+    <t>.064"</t>
+  </si>
+  <si>
+    <t>3/8" 16SWG</t>
+  </si>
+  <si>
+    <t>1/2" 20SWG</t>
+  </si>
+  <si>
+    <t>Gauge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,7 +729,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -706,6 +739,8 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1064,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32:P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1221,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1265,7 +1300,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C5">
         <v>-1500</v>
@@ -1309,43 +1344,43 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1500</v>
+        <v>2600</v>
       </c>
       <c r="E6">
-        <v>750</v>
+        <v>1600</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>-777.19490018076601</v>
+        <v>-1395.31918233285</v>
       </c>
       <c r="H6">
-        <v>-706.02512879588403</v>
+        <v>-1248.59139822629</v>
       </c>
       <c r="I6">
-        <v>1706.86179674289</v>
+        <v>3086.9642233719201</v>
       </c>
       <c r="J6">
-        <v>1571.77546753049</v>
+        <v>2944.2937595571102</v>
       </c>
       <c r="K6">
-        <v>-1092.72384112738</v>
+        <v>-2299.2438749927201</v>
       </c>
       <c r="L6">
-        <v>550.38607294606697</v>
+        <v>976.77524681920704</v>
       </c>
       <c r="M6">
-        <v>874.22629372799304</v>
+        <v>1559.49030448701</v>
       </c>
       <c r="N6">
-        <v>1632.3147029302099</v>
+        <v>2997.5468897268001</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1353,7 +1388,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>-1060</v>
@@ -1397,43 +1432,43 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1500</v>
+        <v>2600</v>
       </c>
       <c r="E8">
-        <v>750</v>
+        <v>1600</v>
       </c>
       <c r="F8">
         <v>-200</v>
       </c>
       <c r="G8">
-        <v>-881.81196821623905</v>
+        <v>-1499.9362503683301</v>
       </c>
       <c r="H8">
-        <v>-660.89656712835597</v>
+        <v>-1203.46283655876</v>
       </c>
       <c r="I8">
-        <v>1518.6123875615699</v>
+        <v>2898.7148141906</v>
       </c>
       <c r="J8">
-        <v>1629.53875908796</v>
+        <v>3002.0570511145902</v>
       </c>
       <c r="K8">
-        <v>-1086.4421433959201</v>
+        <v>-2292.96217726127</v>
       </c>
       <c r="L8">
-        <v>719.46034355487404</v>
+        <v>1145.8495174280099</v>
       </c>
       <c r="M8">
-        <v>924.740843046809</v>
+        <v>1607.9343245687</v>
       </c>
       <c r="N8">
-        <v>1566.26364658588</v>
+        <v>2931.5639406714999</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1441,7 +1476,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>-1060</v>
@@ -1485,7 +1520,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1529,7 +1564,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>-1060</v>
@@ -1573,7 +1608,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1617,7 +1652,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>-1060</v>
@@ -1661,43 +1696,43 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C14">
-        <v>-1500</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>-1500</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>750</v>
+        <v>1350</v>
       </c>
       <c r="F14">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>-881.81196821623905</v>
+        <v>-216.81609908787701</v>
       </c>
       <c r="H14">
-        <v>-1130.45140354091</v>
+        <v>-111.665287410429</v>
       </c>
       <c r="I14">
-        <v>-2613.6894896795502</v>
+        <v>577.81699057906906</v>
       </c>
       <c r="J14">
-        <v>-472.36072167582</v>
+        <v>989.473271269203</v>
       </c>
       <c r="K14">
-        <v>-1092.72384112738</v>
+        <v>-1823.35147667367</v>
       </c>
       <c r="L14">
-        <v>-436.52247104928199</v>
+        <v>102.477241707106</v>
       </c>
       <c r="M14">
-        <v>117.266635243352</v>
+        <v>211.079943438035</v>
       </c>
       <c r="N14">
-        <v>475.76948494638202</v>
+        <v>856.38507290348696</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1705,397 +1740,512 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>-1500</v>
       </c>
       <c r="D15">
-        <v>1500</v>
+        <v>-1500</v>
       </c>
       <c r="E15">
         <v>750</v>
       </c>
       <c r="F15">
+        <v>-200</v>
+      </c>
+      <c r="G15">
+        <v>-1499.9362503683301</v>
+      </c>
+      <c r="H15">
+        <v>-1248.59139822629</v>
+      </c>
+      <c r="I15">
+        <v>-2613.6894896795502</v>
+      </c>
+      <c r="J15">
+        <v>-472.36072167582</v>
+      </c>
+      <c r="K15">
+        <v>-2299.2438749927201</v>
+      </c>
+      <c r="L15">
+        <v>-436.52247104928199</v>
+      </c>
+      <c r="M15">
+        <v>117.266635243352</v>
+      </c>
+      <c r="N15">
+        <v>475.76948494638202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
         <v>0</v>
       </c>
-      <c r="G15">
+      <c r="D16">
+        <v>2600</v>
+      </c>
+      <c r="E16">
+        <v>1600</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>849.74127131781904</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>627.081148896267</v>
       </c>
-      <c r="I15">
-        <v>1706.86179674289</v>
-      </c>
-      <c r="J15">
+      <c r="I16">
+        <v>3086.9642233719201</v>
+      </c>
+      <c r="J16">
         <v>3043.9687055385998</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>-926.94054633412998</v>
       </c>
-      <c r="L15">
-        <v>858.74577703296904</v>
-      </c>
-      <c r="M15">
-        <v>1136.6425941468999</v>
-      </c>
-      <c r="N15">
+      <c r="L16">
+        <v>1145.8495174280099</v>
+      </c>
+      <c r="M16">
+        <v>1607.9343245687</v>
+      </c>
+      <c r="N16">
         <v>4699.7865205453099</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G16" s="9" t="s">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2">
+        <v>210000000000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2">
+        <v>240000000</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2">
-        <v>210000000000</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="2">
-        <v>240000000</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="G20" s="3">
+        <v>275</v>
+      </c>
+      <c r="H20" s="3">
+        <v>278</v>
+      </c>
+      <c r="I20" s="3">
+        <v>391</v>
+      </c>
+      <c r="J20" s="3">
+        <v>436</v>
+      </c>
+      <c r="K20" s="3">
+        <v>584</v>
+      </c>
+      <c r="L20" s="3">
+        <v>329</v>
+      </c>
+      <c r="N20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="3">
+        <f>25.4*3/8</f>
+        <v>9.5249999999999986</v>
+      </c>
+      <c r="H21" s="3">
+        <f>25.4*3/8</f>
+        <v>9.5249999999999986</v>
+      </c>
+      <c r="I21" s="3">
+        <f>25.4*4/8</f>
+        <v>12.7</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" ref="I21:J21" si="0">25.4*3/8</f>
+        <v>9.5249999999999986</v>
+      </c>
+      <c r="K21" s="3">
+        <v>20</v>
+      </c>
+      <c r="L21" s="3">
+        <v>9.5250000000000004</v>
+      </c>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="3">
-        <v>275</v>
-      </c>
-      <c r="H19" s="3">
-        <v>278</v>
-      </c>
-      <c r="I19" s="3">
-        <v>391</v>
-      </c>
-      <c r="J19" s="3">
-        <v>436</v>
-      </c>
-      <c r="K19" s="3">
-        <v>584</v>
-      </c>
-      <c r="L19" s="3">
-        <v>329</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="3">
-        <f>25.4*5/8</f>
-        <v>15.875</v>
-      </c>
-      <c r="H20" s="3">
-        <f t="shared" ref="H20:J20" si="0">25.4*5/8</f>
-        <v>15.875</v>
-      </c>
-      <c r="I20" s="3">
-        <f t="shared" si="0"/>
-        <v>15.875</v>
-      </c>
-      <c r="J20" s="3">
-        <f t="shared" si="0"/>
-        <v>15.875</v>
-      </c>
-      <c r="K20" s="3">
-        <v>10</v>
-      </c>
-      <c r="L20" s="3">
-        <v>10</v>
-      </c>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="4">
-        <f>G20/2000</f>
-        <v>7.9375000000000001E-3</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" ref="H21:L21" si="1">H20/2000</f>
-        <v>7.9375000000000001E-3</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="1"/>
-        <v>7.9375000000000001E-3</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="1"/>
-        <v>7.9375000000000001E-3</v>
-      </c>
-      <c r="K21" s="4">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="L21" s="4">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C22" s="3">
         <v>2</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="5">
-        <f>-G14*(G19/1000)^2/(PI()^2*$C17/$C21)</f>
-        <v>6.4350560218616161E-11</v>
-      </c>
-      <c r="H22" s="5">
-        <f t="shared" ref="H22:L22" si="2">-H14*(H19/1000)^2/(PI()^2*$C17/$C21)</f>
-        <v>8.4304827631150527E-11</v>
-      </c>
-      <c r="I22" s="5">
+        <v>43</v>
+      </c>
+      <c r="G22" s="4">
+        <f>G21/2000</f>
+        <v>4.7624999999999994E-3</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" ref="H22:L22" si="1">H21/2000</f>
+        <v>4.7624999999999994E-3</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="1"/>
+        <v>6.3499999999999997E-3</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="1"/>
+        <v>4.7624999999999994E-3</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="1"/>
+        <v>4.7625000000000002E-3</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="5">
+        <f>-G15*(G20/1000)^2/(PI()^2*$C18/$C22)</f>
+        <v>1.0945841231737897E-10</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" ref="H23:L23" si="2">-H15*(H20/1000)^2/(PI()^2*$C18/$C22)</f>
+        <v>9.3115265529762574E-11</v>
+      </c>
+      <c r="I23" s="5">
         <f t="shared" si="2"/>
         <v>3.8558351830537818E-10</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J23" s="5">
         <f t="shared" si="2"/>
         <v>8.6647834144362775E-11</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K23" s="5">
         <f t="shared" si="2"/>
-        <v>3.596226760506807E-10</v>
-      </c>
-      <c r="L22" s="5">
+        <v>7.5669643518067137E-10</v>
+      </c>
+      <c r="L23" s="5">
         <f t="shared" si="2"/>
         <v>4.5594174433779885E-11</v>
       </c>
-      <c r="N22" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="N23" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="3">
         <v>2</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="7">
-        <f>IF(G22&gt;0,(G21-((-G22+PI() * (G21)^4/4)*4/PI())^0.25)*1000,"Tension only")</f>
-        <v>4.1280088499885681E-2</v>
-      </c>
-      <c r="H23" s="7">
-        <f t="shared" ref="H23:L23" si="3">IF(H22&gt;0,(H21-((-H22+PI() * (H21)^4/4)*4/PI())^0.25)*1000,"Tension only")</f>
-        <v>5.4212970773948738E-2</v>
-      </c>
-      <c r="I23" s="7">
+      <c r="F24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="7">
+        <f>IF(G23&gt;0,(G22-((-G23+PI() * (G22)^4/4)*4/PI())^0.25)*1000,"Tension only")</f>
+        <v>0.36170836774788562</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" ref="H24:L24" si="3">IF(H23&gt;0,(H22-((-H23+PI() * (H22)^4/4)*4/PI())^0.25)*1000,"Tension only")</f>
+        <v>0.30190158314091253</v>
+      </c>
+      <c r="I24" s="7">
         <f t="shared" si="3"/>
-        <v>0.2577050318003215</v>
-      </c>
-      <c r="J23" s="7">
+        <v>0.54575809111232554</v>
+      </c>
+      <c r="J24" s="7">
         <f t="shared" si="3"/>
-        <v>5.5735716678726246E-2</v>
-      </c>
-      <c r="K23" s="7">
+        <v>0.27888490764448742</v>
+      </c>
+      <c r="K24" s="7">
         <f t="shared" si="3"/>
-        <v>1.4045493631664598</v>
-      </c>
-      <c r="L23" s="7">
+        <v>0.25009028757241175</v>
+      </c>
+      <c r="L24" s="7">
         <f t="shared" si="3"/>
-        <v>0.1203828578856857</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="5">
-        <f t="shared" ref="G24:L24" si="4">G15/$C18*$C22</f>
+        <v>0.14044665136541801</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="5">
+        <f>G16/$C19*$C23</f>
         <v>7.0811772609818257E-6</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H25" s="5">
+        <f t="shared" ref="H25:L25" si="4">H16/$C19*$C23</f>
+        <v>5.2256762408022249E-6</v>
+      </c>
+      <c r="I25" s="5">
         <f t="shared" si="4"/>
-        <v>5.2256762408022249E-6</v>
-      </c>
-      <c r="I24" s="5">
-        <f t="shared" si="4"/>
-        <v>1.4223848306190749E-5</v>
-      </c>
-      <c r="J24" s="5">
+        <v>2.5724701861432667E-5</v>
+      </c>
+      <c r="J25" s="5">
         <f t="shared" si="4"/>
         <v>2.5366405879488331E-5</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K25" s="5">
         <f t="shared" si="4"/>
         <v>-7.7245045527844159E-6</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L25" s="5">
         <f t="shared" si="4"/>
-        <v>7.1562148086080753E-6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="7">
-        <f>(G21-(G21^2-G24/PI())^0.5)*1000</f>
-        <v>0.14327793990897164</v>
-      </c>
-      <c r="H25" s="7">
-        <f t="shared" ref="H25:L25" si="5">(H21-(H21^2-H24/PI())^0.5)*1000</f>
-        <v>0.10548098568722089</v>
-      </c>
-      <c r="I25" s="7">
+        <v>9.5487459785667492E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="7">
+        <f>(G22-(G22^2-G25/PI())^0.5)*1000</f>
+        <v>0.24283214472461176</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" ref="H26:L26" si="5">(H22-(H22^2-H25/PI())^0.5)*1000</f>
+        <v>0.17795838272168135</v>
+      </c>
+      <c r="I26" s="7">
         <f t="shared" si="5"/>
-        <v>0.29051924191247047</v>
-      </c>
-      <c r="J25" s="7">
+        <v>0.68130763946609807</v>
+      </c>
+      <c r="J26" s="7">
         <f t="shared" si="5"/>
-        <v>0.52605422460582063</v>
-      </c>
-      <c r="K25" s="7">
+        <v>0.94058575690031621</v>
+      </c>
+      <c r="K26" s="7">
         <f t="shared" si="5"/>
-        <v>-0.24011318246304481</v>
-      </c>
-      <c r="L25" s="7">
+        <v>-0.12219275478505057</v>
+      </c>
+      <c r="L26" s="7">
         <f t="shared" si="5"/>
-        <v>0.23322896723943637</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E26" s="1" t="s">
+        <v>0.33057648933733452</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" ref="G27:L27" si="6">MAX(G26,G24)</f>
+        <v>0.36170836774788562</v>
+      </c>
+      <c r="H27" s="8">
+        <f t="shared" si="6"/>
+        <v>0.30190158314091253</v>
+      </c>
+      <c r="I27" s="8">
+        <f t="shared" si="6"/>
+        <v>0.68130763946609807</v>
+      </c>
+      <c r="J27" s="8">
+        <f t="shared" si="6"/>
+        <v>0.94058575690031621</v>
+      </c>
+      <c r="K27" s="8">
+        <f t="shared" si="6"/>
+        <v>0.25009028757241175</v>
+      </c>
+      <c r="L27" s="8">
+        <f t="shared" si="6"/>
+        <v>0.33057648933733452</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E28" s="9"/>
+      <c r="F28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="8">
-        <f t="shared" ref="G26:L26" si="6">MAX(G25,G23)</f>
-        <v>0.14327793990897164</v>
-      </c>
-      <c r="H26" s="8">
-        <f t="shared" si="6"/>
-        <v>0.10548098568722089</v>
-      </c>
-      <c r="I26" s="8">
-        <f t="shared" si="6"/>
-        <v>0.29051924191247047</v>
-      </c>
-      <c r="J26" s="8">
-        <f t="shared" si="6"/>
-        <v>0.52605422460582063</v>
-      </c>
-      <c r="K26" s="8">
-        <f t="shared" si="6"/>
-        <v>1.4045493631664598</v>
-      </c>
-      <c r="L26" s="8">
-        <f t="shared" si="6"/>
-        <v>0.23322896723943637</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="G28" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="G29" s="6">
-        <f>MAX(ABS(G14),ABS(G15))*$C23</f>
-        <v>1763.6239364324781</v>
-      </c>
-      <c r="H29" s="6">
-        <f t="shared" ref="H29:J29" si="7">MAX(ABS(H14),ABS(H15))*$C23</f>
-        <v>2260.9028070818199</v>
-      </c>
-      <c r="I29" s="6">
+      <c r="G28" s="10">
+        <f>G27/25.4</f>
+        <v>1.4240486919208095E-2</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" ref="H28:L28" si="7">H27/25.4</f>
+        <v>1.1885889100035928E-2</v>
+      </c>
+      <c r="I28" s="10">
         <f t="shared" si="7"/>
+        <v>2.6823135412051106E-2</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="7"/>
+        <v>3.7030935311036073E-2</v>
+      </c>
+      <c r="K28" s="10">
+        <f t="shared" si="7"/>
+        <v>9.8460743138744783E-3</v>
+      </c>
+      <c r="L28" s="10">
+        <f t="shared" si="7"/>
+        <v>1.301482241485569E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G30" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G31" s="6">
+        <f>MAX(ABS(G14),ABS(G15))*$C24</f>
+        <v>2999.8725007366602</v>
+      </c>
+      <c r="H31" s="6">
+        <f>MAX(ABS(H14),ABS(H15))*$C24</f>
+        <v>2497.1827964525801</v>
+      </c>
+      <c r="I31" s="6">
+        <f>MAX(ABS(I14),ABS(I15))*$C24</f>
         <v>5227.3789793591004</v>
       </c>
-      <c r="J29" s="6">
-        <f t="shared" si="7"/>
-        <v>6087.9374110771996</v>
-      </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6">
-        <f>MAX(ABS(M14),ABS(M15))*$C23</f>
-        <v>2273.2851882937998</v>
-      </c>
-      <c r="N29" s="6">
-        <f>MAX(ABS(N14),ABS(N15))*$C23</f>
-        <v>9399.5730410906199</v>
+      <c r="J31" s="6">
+        <f>MAX(ABS(J14),ABS(J15))*$C24</f>
+        <v>1978.946542538406</v>
+      </c>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6">
+        <f>MAX(ABS(M14),ABS(M15))*$C24</f>
+        <v>422.15988687607</v>
+      </c>
+      <c r="N31" s="6">
+        <f>MAX(ABS(N14),ABS(N15))*$C24</f>
+        <v>1712.7701458069739</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>61</v>
+      </c>
+      <c r="P32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
+        <v>57</v>
+      </c>
+      <c r="P34" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G16:N16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G28:N28"/>
+    <mergeCell ref="G17:N17"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G30:N30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>